<commit_message>
Add report folder and materials
</commit_message>
<xml_diff>
--- a/report/table-data/categories.xlsx
+++ b/report/table-data/categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/lm16564_bristol_ac_uk/Documents/Documents/rrr/data-availability-impact/report/table-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="11_F25DC773A252ABDACC1048990958686E5ADE58EC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FF75369D-2FB8-4085-B52D-B3C882CBF987}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="11_F25DC773A252ABDACC1048990958686E5ADE58EC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1EBEBCDB-1851-4377-BF58-AF2DC04866D5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="3675" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Data available</t>
   </si>
@@ -36,18 +36,9 @@
     <t>Data available on request to authors</t>
   </si>
   <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Sub label</t>
-  </si>
-  <si>
     <t>Example</t>
   </si>
   <si>
-    <t>Data available from central repository (requires sufficient details to identify e.g. extract ID. For example: acceptable )</t>
-  </si>
-  <si>
     <t>"Data sharing not applicable to this article as no datasets were generated or analysed during the current study."[@ehrlich2019]</t>
   </si>
   <si>
@@ -76,6 +67,30 @@
   </si>
   <si>
     <t>Not applicable (protocol for a review, commentary, etc)</t>
+  </si>
+  <si>
+    <t>Data will be available in the future</t>
+  </si>
+  <si>
+    <t>Data vailable from central repository, but insufficient detail published to find</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>"Data were obtained from the international MSBase cohort study. Information regarding data availability can be obtained at https://www.msbase.org/."[@malpas2019]</t>
+  </si>
+  <si>
+    <t>"The protocol and full dataset will be available at Open Science Framework upon peer review publication (https://osf.io/rvbuy/)."[@ebbeling2019]</t>
+  </si>
+  <si>
+    <t>Main category</t>
+  </si>
+  <si>
+    <t>Sub-category</t>
+  </si>
+  <si>
+    <t>Data available from central repository (requires sufficient details to identify e.g. extract or accession ID)</t>
   </si>
 </sst>
 </file>
@@ -111,8 +126,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,93 +411,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Range of updates to report/report data
</commit_message>
<xml_diff>
--- a/report/table-data/categories.xlsx
+++ b/report/table-data/categories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/lm16564_bristol_ac_uk/Documents/Documents/rrr/data-availability-impact/report/table-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="11_F25DC773A252ABDACC1048990958686E5ADE58EC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1EBEBCDB-1851-4377-BF58-AF2DC04866D5}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="11_F25DC773A252ABDACC1048990958686E5ADE58EC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B18C075A-2889-437C-BFCC-9D253A39EE7D}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="3675" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25980" yWindow="5325" windowWidth="2400" windowHeight="585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Data available</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Data available from central repository (requires sufficient details to identify e.g. extract or accession ID)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -411,38 +414,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
-    <col min="3" max="3" width="55" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="55" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -452,10 +458,10 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
@@ -466,10 +472,10 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
@@ -480,24 +486,24 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
@@ -508,10 +514,10 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
@@ -522,32 +528,29 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Remove GitHub from examples
</commit_message>
<xml_diff>
--- a/report/table-data/categories.xlsx
+++ b/report/table-data/categories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/lm16564_bristol_ac_uk/Documents/Documents/rrr/data-availability-impact/report/table-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="181" documentId="11_F25DC773A252ABDACC1048990958686E5ADE58EC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2D7D469A-5506-4541-87C1-BDE49B0F6A1A}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="11_F25DC773A252ABDACC1048990958686E5ADE58EC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EDD363CD-5A12-4410-9A84-1531EC7836A3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>"Open"</t>
   </si>
   <si>
-    <t>Data available via a online repository that is not access-controlled e.g. GitHub, Zenodo</t>
-  </si>
-  <si>
     <t>Data will be made available in the future (link provided)</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>@barry2020</t>
+  </si>
+  <si>
+    <t>Data available via a online repository that is not access-controlled e.g. Dryad, Zenodo</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +479,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -493,10 +493,10 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -510,10 +510,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -527,10 +527,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -541,13 +541,13 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -558,13 +558,13 @@
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -575,13 +575,13 @@
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -592,13 +592,13 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -612,10 +612,10 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -626,13 +626,13 @@
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>